<commit_message>
export đơn hàng trực tiếp
</commit_message>
<xml_diff>
--- a/DMS/Templates/Indirect_Order_Export.xlsx
+++ b/DMS/Templates/Indirect_Order_Export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E01ED9D-C2CA-4811-B5A5-7BC03A9372C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849ACAE9-B881-431A-89EC-9A8B88609157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -238,6 +238,43 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -267,50 +304,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,7 +632,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,114 +653,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
-    <row r="4" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="8"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
-    <row r="7" spans="1:13" s="13" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:13" s="8" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="19"/>
     </row>
     <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -767,16 +805,16 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="1" t="s">
         <v>30</v>
       </c>
@@ -786,17 +824,17 @@
       <c r="K10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="19"/>
-      <c r="M10" s="16"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A4:K4"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A8:K8"/>
     <mergeCell ref="E5:H5"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>